<commit_message>
Added DNA and PCR concentrations
</commit_message>
<xml_diff>
--- a/metaprobe_DNA_and_PCR_record.xlsx
+++ b/metaprobe_DNA_and_PCR_record.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://365abdn-my.sharepoint.com/personal/r01er21_abdn_ac_uk/Documents/Chapter 3 Metaprobe results/Chapter_3_seagrass_BRUV_metaprobes_GIT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{F8F8E060-CEB4-4661-8667-CC2912750641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A79A3B09-4560-443E-A094-697AA2831FFE}"/>
+  <xr:revisionPtr revIDLastSave="123" documentId="8_{F8F8E060-CEB4-4661-8667-CC2912750641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A323C891-82F0-4C1B-9A41-D756782705D5}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AB0F6F0B-7428-401F-A883-883AFFD73786}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{AB0F6F0B-7428-401F-A883-883AFFD73786}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="for_r_plot" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="62">
   <si>
     <t>Sample ID</t>
   </si>
@@ -204,6 +205,24 @@
   </si>
   <si>
     <t>MiFishU replicate iii</t>
+  </si>
+  <si>
+    <t>Sample_ID</t>
+  </si>
+  <si>
+    <t>Gauze</t>
+  </si>
+  <si>
+    <t>Pooled_Tele02</t>
+  </si>
+  <si>
+    <t>Pooled_MiFishU</t>
+  </si>
+  <si>
+    <t>Probe</t>
+  </si>
+  <si>
+    <t>Deployment</t>
   </si>
 </sst>
 </file>
@@ -211,7 +230,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -711,29 +730,29 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -754,6 +773,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1075,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FE8153-2D90-476E-9902-3541EE243F33}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2377,4 +2400,768 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D21004C-8E6D-4620-A1DD-6111E21208CE}">
+  <dimension ref="A1:F39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="49">
+        <v>0.11</v>
+      </c>
+      <c r="E2" s="49">
+        <v>1.58</v>
+      </c>
+      <c r="F2" s="49">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="50">
+        <v>7.6799999999999993E-2</v>
+      </c>
+      <c r="E3" s="50">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="F3" s="50">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="50">
+        <v>9.1600000000000001E-2</v>
+      </c>
+      <c r="E4" s="50">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="F4" s="50">
+        <v>0.29599999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="50">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="E5" s="50">
+        <v>1.65</v>
+      </c>
+      <c r="F5" s="50">
+        <v>0.41199999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2</v>
+      </c>
+      <c r="D6" s="50">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="50">
+        <v>7.3599999999999999E-2</v>
+      </c>
+      <c r="E7" s="50">
+        <v>2.96</v>
+      </c>
+      <c r="F7" s="50">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>3</v>
+      </c>
+      <c r="D8" s="50">
+        <v>0.13</v>
+      </c>
+      <c r="E8" s="50">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="F8" s="50">
+        <v>0.32200000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" s="50">
+        <v>0.13</v>
+      </c>
+      <c r="E9" s="50">
+        <v>1.61</v>
+      </c>
+      <c r="F9" s="50">
+        <v>0.54400000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
+      </c>
+      <c r="D10" s="52">
+        <v>0.129</v>
+      </c>
+      <c r="E10" s="52">
+        <v>1.62</v>
+      </c>
+      <c r="F10" s="52">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4</v>
+      </c>
+      <c r="D11" s="49">
+        <v>9.8799999999999999E-2</v>
+      </c>
+      <c r="E11" s="49">
+        <v>3.22</v>
+      </c>
+      <c r="F11" s="49">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>4</v>
+      </c>
+      <c r="D12" s="50">
+        <v>9.4399999999999998E-2</v>
+      </c>
+      <c r="E12" s="50">
+        <v>4.16</v>
+      </c>
+      <c r="F12" s="50">
+        <v>1.18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>4</v>
+      </c>
+      <c r="D13" s="50">
+        <v>0.105</v>
+      </c>
+      <c r="E13" s="50">
+        <v>2.04</v>
+      </c>
+      <c r="F13" s="50">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2">
+        <v>5</v>
+      </c>
+      <c r="D14" s="50">
+        <v>0.1</v>
+      </c>
+      <c r="E14" s="50">
+        <v>1.9</v>
+      </c>
+      <c r="F14" s="50">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>5</v>
+      </c>
+      <c r="D15" s="50">
+        <v>9.5600000000000004E-2</v>
+      </c>
+      <c r="E15" s="50">
+        <v>2.68</v>
+      </c>
+      <c r="F15" s="50">
+        <v>0.63200000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2</v>
+      </c>
+      <c r="C16" s="2">
+        <v>5</v>
+      </c>
+      <c r="D16" s="50">
+        <v>8.3599999999999994E-2</v>
+      </c>
+      <c r="E16" s="50">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="F16" s="50">
+        <v>0.17399999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2">
+        <v>6</v>
+      </c>
+      <c r="D17" s="50">
+        <v>8.2799999999999999E-2</v>
+      </c>
+      <c r="E17" s="50">
+        <v>11.1</v>
+      </c>
+      <c r="F17" s="50">
+        <v>0.81799999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2</v>
+      </c>
+      <c r="C18" s="2">
+        <v>6</v>
+      </c>
+      <c r="D18" s="50">
+        <v>0.109</v>
+      </c>
+      <c r="E18" s="50">
+        <v>1.99</v>
+      </c>
+      <c r="F18" s="50">
+        <v>0.60599999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2</v>
+      </c>
+      <c r="C19" s="3">
+        <v>6</v>
+      </c>
+      <c r="D19" s="52">
+        <v>6.6799999999999998E-2</v>
+      </c>
+      <c r="E19" s="52">
+        <v>1.7</v>
+      </c>
+      <c r="F19" s="52">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1">
+        <v>7</v>
+      </c>
+      <c r="D20" s="49">
+        <v>0.121</v>
+      </c>
+      <c r="E20" s="49">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="F20" s="49">
+        <v>0.216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>3</v>
+      </c>
+      <c r="C21" s="2">
+        <v>7</v>
+      </c>
+      <c r="D21" s="50">
+        <v>7.1599999999999997E-2</v>
+      </c>
+      <c r="E21" s="50">
+        <v>0.96799999999999997</v>
+      </c>
+      <c r="F21" s="50">
+        <v>0.41399999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2">
+        <v>7</v>
+      </c>
+      <c r="D22" s="50">
+        <v>5.2400000000000002E-2</v>
+      </c>
+      <c r="E22" s="50">
+        <v>0.216</v>
+      </c>
+      <c r="F22" s="50">
+        <v>0.13400000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>3</v>
+      </c>
+      <c r="C23" s="2">
+        <v>8</v>
+      </c>
+      <c r="D23" s="50">
+        <v>8.1199999999999994E-2</v>
+      </c>
+      <c r="E23" s="50">
+        <v>1.97</v>
+      </c>
+      <c r="F23" s="50">
+        <v>0.312</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2">
+        <v>8</v>
+      </c>
+      <c r="D24" s="50">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="E24" s="50">
+        <v>0.79</v>
+      </c>
+      <c r="F24" s="50">
+        <v>0.34200000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>3</v>
+      </c>
+      <c r="C25" s="2">
+        <v>8</v>
+      </c>
+      <c r="D25" s="50">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="E25" s="50">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="F25" s="50">
+        <v>0.64400000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2">
+        <v>9</v>
+      </c>
+      <c r="D26" s="50">
+        <v>0.126</v>
+      </c>
+      <c r="E26" s="50">
+        <v>2.02</v>
+      </c>
+      <c r="F26" s="50">
+        <v>0.14199999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2">
+        <v>9</v>
+      </c>
+      <c r="D27" s="50">
+        <v>0.155</v>
+      </c>
+      <c r="E27" s="50">
+        <v>4.54</v>
+      </c>
+      <c r="F27" s="50">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>3</v>
+      </c>
+      <c r="C28" s="3">
+        <v>9</v>
+      </c>
+      <c r="D28" s="52">
+        <v>0.193</v>
+      </c>
+      <c r="E28" s="52">
+        <v>3.24</v>
+      </c>
+      <c r="F28" s="52">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1">
+        <v>10</v>
+      </c>
+      <c r="D29" s="49">
+        <v>9.3200000000000005E-2</v>
+      </c>
+      <c r="E29" s="49">
+        <v>1.28</v>
+      </c>
+      <c r="F29" s="49">
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>4</v>
+      </c>
+      <c r="C30" s="2">
+        <v>10</v>
+      </c>
+      <c r="D30" s="50">
+        <v>0.151</v>
+      </c>
+      <c r="E30" s="50">
+        <v>1.23</v>
+      </c>
+      <c r="F30" s="50">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>4</v>
+      </c>
+      <c r="C31" s="2">
+        <v>10</v>
+      </c>
+      <c r="D31" s="50">
+        <v>0.121</v>
+      </c>
+      <c r="E31" s="50">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="F31" s="50">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1">
+        <v>4</v>
+      </c>
+      <c r="C32" s="2">
+        <v>11</v>
+      </c>
+      <c r="D32" s="50">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="E32" s="50">
+        <v>1</v>
+      </c>
+      <c r="F32" s="50">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2">
+        <v>4</v>
+      </c>
+      <c r="C33" s="2">
+        <v>11</v>
+      </c>
+      <c r="D33" s="50">
+        <v>0.106</v>
+      </c>
+      <c r="E33" s="50">
+        <v>3.16</v>
+      </c>
+      <c r="F33" s="50">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2">
+        <v>4</v>
+      </c>
+      <c r="C34" s="2">
+        <v>11</v>
+      </c>
+      <c r="D34" s="50">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="E34" s="50">
+        <v>2.54</v>
+      </c>
+      <c r="F34" s="50">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1">
+        <v>4</v>
+      </c>
+      <c r="C35" s="2">
+        <v>12</v>
+      </c>
+      <c r="D35" s="50">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="E35" s="50">
+        <v>0.59</v>
+      </c>
+      <c r="F35" s="50">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2">
+        <v>4</v>
+      </c>
+      <c r="C36" s="2">
+        <v>12</v>
+      </c>
+      <c r="D36" s="50">
+        <v>9.7600000000000006E-2</v>
+      </c>
+      <c r="E36" s="50">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="F36" s="50">
+        <v>0.34599999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>4</v>
+      </c>
+      <c r="C37" s="3">
+        <v>12</v>
+      </c>
+      <c r="D37" s="52">
+        <v>0.189</v>
+      </c>
+      <c r="E37" s="52">
+        <v>1.52</v>
+      </c>
+      <c r="F37" s="52">
+        <v>0.222</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D38" s="59"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D39" s="59"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>